<commit_message>
All basic formulas excel
</commit_message>
<xml_diff>
--- a/Excel/Project Work/Formula.xlsx
+++ b/Excel/Project Work/Formula.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Practice Project\data science\data-analysis\Excel\Project Work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Data Science\data-analysis\Excel\Project Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EDF544-8DC1-4D3E-BD5A-F4549BD07E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Max-Min" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
     <sheet name="Concatenate" sheetId="10" r:id="rId10"/>
     <sheet name="Days-NetworkDays" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -44,14 +43,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -66,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="91">
   <si>
     <t>EmployeeID</t>
   </si>
@@ -334,11 +333,17 @@
   <si>
     <t>Date(conversion)</t>
   </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
@@ -602,7 +607,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
@@ -1911,13 +1916,15 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1932,7 +1939,7 @@
     <col min="11" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1963,8 +1970,14 @@
       <c r="J1" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1001</v>
       </c>
@@ -1992,8 +2005,12 @@
       <c r="I2" s="2">
         <v>42253</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" t="str">
+        <f>CONCATENATE(B2:B10," ",C2:C10)</f>
+        <v>Jim Halpert</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1002</v>
       </c>
@@ -2021,8 +2038,12 @@
       <c r="I3" s="2">
         <v>42287</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J10" si="0">CONCATENATE(B3:B11," ",C3:C11)</f>
+        <v>Pam Beasley</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1003</v>
       </c>
@@ -2050,8 +2071,12 @@
       <c r="I4" s="2">
         <v>42986</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>Dwight Schrute</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1004</v>
       </c>
@@ -2079,8 +2104,12 @@
       <c r="I5" s="2">
         <v>42341</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>Angela Martin</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1005</v>
       </c>
@@ -2108,8 +2137,12 @@
       <c r="I6" s="2">
         <v>42977</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>Toby Flenderson</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1006</v>
       </c>
@@ -2137,8 +2170,12 @@
       <c r="I7" s="2">
         <v>41528</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>Michael Scott</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1007</v>
       </c>
@@ -2166,8 +2203,12 @@
       <c r="I8" s="2">
         <v>41551</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>Meredith Palmer</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1008</v>
       </c>
@@ -2195,8 +2236,12 @@
       <c r="I9" s="2">
         <v>42116</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>Stanley Hudson</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1009</v>
       </c>
@@ -2224,16 +2269,20 @@
       <c r="I10" s="2">
         <v>40800</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>Kevin Malone</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H11" s="1" t="str">
-        <f t="shared" ref="H11:H12" si="0">CONCATENATE(B11," ",C11)</f>
+        <f t="shared" ref="H11:H12" si="1">CONCATENATE(B11," ",C11)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H12" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3224,13 +3273,15 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3303,6 +3354,14 @@
       <c r="I2" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="J2">
+        <f>_xlfn.DAYS(I2,H2)</f>
+        <v>5056</v>
+      </c>
+      <c r="K2">
+        <f>NETWORKDAYS(H2,I2)</f>
+        <v>3611</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -3332,6 +3391,14 @@
       <c r="I3" s="5" t="s">
         <v>48</v>
       </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J10" si="0">_xlfn.DAYS(I3,H3)</f>
+        <v>5851</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K10" si="1">NETWORKDAYS(H3,I3)</f>
+        <v>4180</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -3361,6 +3428,14 @@
       <c r="I4" s="5" t="s">
         <v>51</v>
       </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>6275</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>4484</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -3390,6 +3465,14 @@
       <c r="I5" s="5" t="s">
         <v>54</v>
       </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>5811</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>4152</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -3419,6 +3502,14 @@
       <c r="I6" s="5" t="s">
         <v>57</v>
       </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>5960</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>4258</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -3448,6 +3539,14 @@
       <c r="I7" s="5" t="s">
         <v>59</v>
       </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>4511</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>3223</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -3477,6 +3576,14 @@
       <c r="I8" s="5" t="s">
         <v>59</v>
       </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>3595</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>2568</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -3506,6 +3613,14 @@
       <c r="I9" s="5" t="s">
         <v>64</v>
       </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>4700</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>3358</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -3534,6 +3649,14 @@
       </c>
       <c r="I10" s="5" t="s">
         <v>64</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>4273</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>3053</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4523,7 +4646,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
@@ -4609,7 +4732,7 @@
         <v>Young</v>
       </c>
       <c r="K2" s="1" t="e">
-        <f t="shared" ref="K2:K10" ca="1" si="1">_xludf.ifs(F2:F10="Salesman", "Sales", F2:F10="HR", "Fire Him", F2:F10="Accountant","Give Bonus")</f>
+        <f t="shared" ref="K2:K10" ca="1" si="1">ifs(F2:F10="Salesman", "Sales", F2:F10="HR", "Fire Him", F2:F10="Accountant","Give Bonus")</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -5896,7 +6019,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
@@ -7231,7 +7354,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
@@ -8650,13 +8773,13 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
@@ -10013,13 +10136,15 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10092,6 +10217,10 @@
       <c r="I2" s="2">
         <v>42253</v>
       </c>
+      <c r="J2" t="str">
+        <f>TRIM(C2:C10)</f>
+        <v>Halpert</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -10121,6 +10250,10 @@
       <c r="I3" s="2">
         <v>42287</v>
       </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J10" si="0">TRIM(C3:C11)</f>
+        <v>Beasley</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -10150,6 +10283,10 @@
       <c r="I4" s="2">
         <v>42986</v>
       </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>Schrute</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -10179,6 +10316,10 @@
       <c r="I5" s="2">
         <v>42341</v>
       </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>Martin</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -10208,6 +10349,10 @@
       <c r="I6" s="2">
         <v>42977</v>
       </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>Flenderson</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -10237,6 +10382,10 @@
       <c r="I7" s="2">
         <v>41528</v>
       </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>Scott</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -10266,6 +10415,10 @@
       <c r="I8" s="2">
         <v>41551</v>
       </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>Palmer</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -10295,6 +10448,10 @@
       <c r="I9" s="2">
         <v>42116</v>
       </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>Hudson</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -10323,6 +10480,10 @@
       </c>
       <c r="I10" s="2">
         <v>40800</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>Malone</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11312,13 +11473,15 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11394,6 +11557,18 @@
       <c r="I2" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="J2" t="str">
+        <f>SUBSTITUTE(H2:H10,"/","-",1)</f>
+        <v>11-2/2001</v>
+      </c>
+      <c r="K2" t="str">
+        <f>SUBSTITUTE(I2:I10,"/","-",2)</f>
+        <v>9/6-2015</v>
+      </c>
+      <c r="L2" t="str">
+        <f>SUBSTITUTE(H2:H10, "/", "-")</f>
+        <v>11-2-2001</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -11423,6 +11598,18 @@
       <c r="I3" s="5" t="s">
         <v>48</v>
       </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J10" si="0">SUBSTITUTE(H3:H11,"/","-",1)</f>
+        <v>10-3/1999</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K10" si="1">SUBSTITUTE(I3:I11,"/","-",2)</f>
+        <v>10/10-2015</v>
+      </c>
+      <c r="L3" t="str">
+        <f>SUBSTITUTE(H3:H11, "/", "-")</f>
+        <v>10-3-1999</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -11452,6 +11639,18 @@
       <c r="I4" s="5" t="s">
         <v>51</v>
       </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>7-4/2000</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="1"/>
+        <v>9/8-2017</v>
+      </c>
+      <c r="L4" t="str">
+        <f>SUBSTITUTE(H4:H12, "/", "-")</f>
+        <v>7-4-2000</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -11481,6 +11680,18 @@
       <c r="I5" s="5" t="s">
         <v>54</v>
       </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>1-5/2000</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>12/3-2015</v>
+      </c>
+      <c r="L5" t="str">
+        <f>SUBSTITUTE(H5:H13, "/", "-")</f>
+        <v>1-5-2000</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -11510,6 +11721,18 @@
       <c r="I6" s="5" t="s">
         <v>57</v>
       </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>5-6/2001</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>8/30-2017</v>
+      </c>
+      <c r="L6" t="str">
+        <f>SUBSTITUTE(H6:H14, "/", "-")</f>
+        <v>5-6-2001</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -11539,6 +11762,18 @@
       <c r="I7" s="5" t="s">
         <v>59</v>
       </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>5-6/2001</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>9/11-2013</v>
+      </c>
+      <c r="L7" t="str">
+        <f>SUBSTITUTE(H7:H15, "/", "-")</f>
+        <v>5-6-2001</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -11568,6 +11803,18 @@
       <c r="I8" s="5" t="s">
         <v>59</v>
       </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>11-8/2003</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>9/11-2013</v>
+      </c>
+      <c r="L8" t="str">
+        <f>SUBSTITUTE(H8:H16, "/", "-")</f>
+        <v>11-8-2003</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -11597,6 +11844,18 @@
       <c r="I9" s="5" t="s">
         <v>64</v>
       </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>6-9/2002</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>4/22-2015</v>
+      </c>
+      <c r="L9" t="str">
+        <f>SUBSTITUTE(H9:H17, "/", "-")</f>
+        <v>6-9-2002</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -11625,6 +11884,18 @@
       </c>
       <c r="I10" s="5" t="s">
         <v>64</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>8-10/2003</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>4/22-2015</v>
+      </c>
+      <c r="L10" t="str">
+        <f>SUBSTITUTE(H10:H18, "/", "-")</f>
+        <v>8-10-2003</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -14622,20 +14893,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:L1000"/>
+  <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="26" width="13" customWidth="1"/>
+    <col min="1" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="27.85546875" customWidth="1"/>
+    <col min="14" max="27" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14666,14 +14941,15 @@
       <c r="J1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="1"/>
+      <c r="L1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1001</v>
       </c>
@@ -14701,8 +14977,24 @@
       <c r="I2" s="2">
         <v>42253</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <f>SUM(G2:G10)</f>
+        <v>437000</v>
+      </c>
+      <c r="K2">
+        <f>SUMIF(D2:D10,"&lt;30", G2:G10)</f>
+        <v>63000</v>
+      </c>
+      <c r="L2">
+        <f>SUMIF(D2:D10,"&gt;30", G2:G10)</f>
+        <v>293000</v>
+      </c>
+      <c r="M2">
+        <f>SUMIFS(G2:G10,E2:E10,"Female",D2:D10,"&gt;30")</f>
+        <v>88000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1002</v>
       </c>
@@ -14730,8 +15022,12 @@
       <c r="I3" s="2">
         <v>42287</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <f>SUM(K2,L2)</f>
+        <v>356000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1003</v>
       </c>
@@ -14759,8 +15055,12 @@
       <c r="I4" s="2">
         <v>42986</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <f>SUMIF(D2:D10,"30", G2:G10)</f>
+        <v>81000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1004</v>
       </c>
@@ -14788,8 +15088,12 @@
       <c r="I5" s="2">
         <v>42341</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <f>SUM(K3,K4)</f>
+        <v>437000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1005</v>
       </c>
@@ -14818,7 +15122,7 @@
         <v>42977</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1006</v>
       </c>
@@ -14847,7 +15151,7 @@
         <v>41528</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1007</v>
       </c>
@@ -14876,7 +15180,7 @@
         <v>41551</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1008</v>
       </c>
@@ -14905,7 +15209,7 @@
         <v>42116</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1009</v>
       </c>
@@ -15921,13 +16225,15 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16002,6 +16308,18 @@
       </c>
       <c r="I2" s="2">
         <v>42253</v>
+      </c>
+      <c r="J2">
+        <f>COUNT(D2:D10)</f>
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <f>COUNTIF(G2:G10, "&gt;40000")</f>
+        <v>8</v>
+      </c>
+      <c r="L2">
+        <f>COUNTIFS(D2:D10, "&gt;30", E2:E10, "Male")</f>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>